<commit_message>
new change to office branch
</commit_message>
<xml_diff>
--- a/CR.xlsx
+++ b/CR.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/test_site/learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34624F35-BC0D-5E43-9744-4B62BCBF0012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87960E1-049F-2743-B5C0-582CBC036E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14400" xr2:uid="{1CEF2A5D-585A-3643-AFFB-79860CDE4BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Backup Description </t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>The last time I did not complete it</t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -130,10 +133,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6563AF53-C039-3740-A9E8-2447F09899BF}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,62 +472,62 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <f ca="1">TODAY()+2</f>
-        <v>44883</v>
+        <v>44889</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f ca="1">B6+1</f>
-        <v>44884</v>
+        <v>44890</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -537,14 +540,19 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>